<commit_message>
Collapse. expand sidebar menu, filter popup
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -12,7 +12,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+  <si>
+    <t>Mã Sp</t>
+  </si>
+  <si>
+    <t>Tên Sp</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Tình trạng</t>
+  </si>
   <si>
     <t>1</t>
   </si>
@@ -41,21 +56,6 @@
     <t>vdsfd</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>sdvdsvsx</t>
-  </si>
-  <si>
-    <t>678</t>
-  </si>
-  <si>
-    <t>dfvfv</t>
-  </si>
-  <si>
-    <t>Ngưng kinh doanh</t>
-  </si>
-  <si>
     <t>4</t>
   </si>
   <si>
@@ -63,18 +63,6 @@
   </si>
   <si>
     <t>444</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>fhfdgdf</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
   </si>
 </sst>
 </file>
@@ -120,7 +108,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -157,24 +145,24 @@
         <v>8</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -188,27 +176,10 @@
         <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>